<commit_message>
minor update from Alison on geometry mapping reference file
</commit_message>
<xml_diff>
--- a/wwpdb/utils/dp/metal/metal_ref/coord_classes_mapping_abbr.xlsx
+++ b/wwpdb/utils/dp/metal/metal_ref/coord_classes_mapping_abbr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abiester/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abiester/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AE64A6-5FF8-DA4B-AB02-9C5F79A31797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E9E0EB-BF0E-7648-9899-EA411A03BFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="760" windowWidth="25520" windowHeight="20360" tabRatio="215" xr2:uid="{CE4FFC7F-553B-A742-BB60-E7102764A25A}"/>
+    <workbookView xWindow="9040" yWindow="760" windowWidth="25520" windowHeight="20280" tabRatio="215" xr2:uid="{CE4FFC7F-553B-A742-BB60-E7102764A25A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,18 +194,6 @@
     <t>pentagonal bipyramid with a vacancy (equatorial)</t>
   </si>
   <si>
-    <t>octahedron, face monocapped with a vacancy (capped face)</t>
-  </si>
-  <si>
-    <t>octahedron, face monocapped with a vacancy (non-capped face)</t>
-  </si>
-  <si>
-    <t>trigonal prism, square-face monocapped with a vacancy (capped face)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trigonal prism, square-face monocapped with a vacancy (non-capped edge)	</t>
-  </si>
-  <si>
     <t>sandwich_4h_2</t>
   </si>
   <si>
@@ -245,15 +233,9 @@
     <t>pentagonal bipyramidal</t>
   </si>
   <si>
-    <t>trigonal prism, square-face monocapped</t>
-  </si>
-  <si>
     <t>capped-trigonal-prism</t>
   </si>
   <si>
-    <t>octahedron, face monocapped</t>
-  </si>
-  <si>
     <t>hexagonal bipyramid with a vacancy (axial)</t>
   </si>
   <si>
@@ -323,15 +305,6 @@
     <t>square antiprismatic</t>
   </si>
   <si>
-    <t>octahedron, trans-bicapped</t>
-  </si>
-  <si>
-    <t>trigonal prism, square-face bicapped</t>
-  </si>
-  <si>
-    <t>trigonal prism, triangular-face bicapped</t>
-  </si>
-  <si>
     <t>elongated-triangular-bipyramid</t>
   </si>
   <si>
@@ -383,15 +356,9 @@
     <t>dodecahedral</t>
   </si>
   <si>
-    <t>trigonal prism, square-face tricapped</t>
-  </si>
-  <si>
     <t>tricapped-trigonal-prismatic</t>
   </si>
   <si>
-    <t>square antiprism, square-face monocapped</t>
-  </si>
-  <si>
     <t>sandwich_7_2</t>
   </si>
   <si>
@@ -1095,6 +1062,39 @@
   </si>
   <si>
     <t>PTR</t>
+  </si>
+  <si>
+    <t>octahedron face monocapped with a vacancy (capped face)</t>
+  </si>
+  <si>
+    <t>octahedron face monocapped with a vacancy (non-capped face)</t>
+  </si>
+  <si>
+    <t>trigonal prism square-face monocapped with a vacancy (capped face)</t>
+  </si>
+  <si>
+    <t>square antiprism square-face monocapped</t>
+  </si>
+  <si>
+    <t>trigonal prism square-face tricapped</t>
+  </si>
+  <si>
+    <t>trigonal prism square-face bicapped</t>
+  </si>
+  <si>
+    <t>trigonal prism triangular-face bicapped</t>
+  </si>
+  <si>
+    <t>octahedron trans-bicapped</t>
+  </si>
+  <si>
+    <t>trigonal prism square-face monocapped</t>
+  </si>
+  <si>
+    <t>octahedron face monocapped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trigonal prism square-face monocapped with a vacancy (non-capped edge)	</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EFD5C9-5AC4-344D-9544-09553ED94A47}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="126" zoomScaleNormal="211" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="126" zoomScaleNormal="211" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1551,13 +1551,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1571,13 +1571,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1591,13 +1591,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1611,13 +1611,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1631,19 +1631,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1651,13 +1651,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1677,7 +1677,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -1691,13 +1691,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -1711,13 +1711,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1731,13 +1731,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1751,7 +1751,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1763,7 +1763,7 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -1771,7 +1771,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -1783,7 +1783,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1797,7 +1797,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
@@ -1817,7 +1817,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -1837,13 +1837,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -1851,13 +1851,13 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -1871,13 +1871,13 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -1891,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1917,7 +1917,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1937,7 +1937,7 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E20" t="s">
         <v>42</v>
@@ -1957,7 +1957,7 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
@@ -1971,13 +1971,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -1991,13 +1991,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="E23" t="s">
         <v>49</v>
@@ -2011,7 +2011,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -2023,7 +2023,7 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -2031,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -2043,7 +2043,7 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -2051,10 +2051,10 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>343</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -2063,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -2071,10 +2071,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -2083,7 +2083,7 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -2091,10 +2091,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>345</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -2103,7 +2103,7 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -2111,10 +2111,10 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>353</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
@@ -2123,7 +2123,7 @@
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -2137,13 +2137,13 @@
         <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -2157,13 +2157,13 @@
         <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -2177,13 +2177,13 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -2197,13 +2197,13 @@
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -2217,13 +2217,13 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -2231,19 +2231,19 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="E35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -2251,19 +2251,19 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>351</v>
       </c>
       <c r="D36" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
@@ -2271,10 +2271,10 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>352</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
@@ -2283,7 +2283,7 @@
         <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -2291,10 +2291,10 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
@@ -2303,7 +2303,7 @@
         <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -2311,10 +2311,10 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -2323,7 +2323,7 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -2331,10 +2331,10 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -2343,7 +2343,7 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -2351,10 +2351,10 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
         <v>14</v>
@@ -2363,7 +2363,7 @@
         <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -2377,13 +2377,13 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F42" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -2397,13 +2397,13 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
@@ -2417,13 +2417,13 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -2437,13 +2437,13 @@
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -2457,13 +2457,13 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="E46" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F46" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -2471,19 +2471,19 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="E47" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -2491,19 +2491,19 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F48" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -2511,19 +2511,19 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D49" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -2531,10 +2531,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>350</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>
@@ -2543,7 +2543,7 @@
         <v>14</v>
       </c>
       <c r="F50" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -2551,10 +2551,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>348</v>
       </c>
       <c r="D51" t="s">
         <v>14</v>
@@ -2563,7 +2563,7 @@
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -2571,19 +2571,19 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>349</v>
       </c>
       <c r="D52" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="E52" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -2597,13 +2597,13 @@
         <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E53" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F53" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
@@ -2617,13 +2617,13 @@
         <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -2637,13 +2637,13 @@
         <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F55" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -2657,13 +2657,13 @@
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="E56" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F56" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -2677,13 +2677,13 @@
         <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F57" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -2697,13 +2697,13 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="E58" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F58" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -2717,13 +2717,13 @@
         <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="E59" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F59" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -2737,13 +2737,13 @@
         <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="E60" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -2757,13 +2757,13 @@
         <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F61" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -2771,19 +2771,19 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>347</v>
       </c>
       <c r="D62" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="E62" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F62" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
@@ -2791,10 +2791,10 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>346</v>
       </c>
       <c r="D63" t="s">
         <v>14</v>
@@ -2803,7 +2803,7 @@
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
@@ -2817,13 +2817,13 @@
         <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="E64" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F64" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
@@ -2837,13 +2837,13 @@
         <v>14</v>
       </c>
       <c r="D65" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="E65" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F65" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
@@ -2857,13 +2857,13 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E66" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F66" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -2877,13 +2877,13 @@
         <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F67" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
@@ -2897,13 +2897,13 @@
         <v>14</v>
       </c>
       <c r="D68" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E68" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F68" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
@@ -2917,13 +2917,13 @@
         <v>14</v>
       </c>
       <c r="D69" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="E69" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F69" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -2937,13 +2937,13 @@
         <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E70" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F70" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
@@ -2957,13 +2957,13 @@
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F71" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
@@ -2977,13 +2977,13 @@
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E72" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F72" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
@@ -2997,13 +2997,13 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E73" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F73" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
@@ -3017,13 +3017,13 @@
         <v>14</v>
       </c>
       <c r="D74" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F74" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
@@ -3037,13 +3037,13 @@
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="E75" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F75" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
@@ -3057,13 +3057,13 @@
         <v>14</v>
       </c>
       <c r="D76" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="F76" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
@@ -3077,13 +3077,13 @@
         <v>14</v>
       </c>
       <c r="D77" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F77" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
@@ -3097,13 +3097,13 @@
         <v>14</v>
       </c>
       <c r="D78" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E78" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F78" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
@@ -3117,13 +3117,13 @@
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="E79" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F79" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
@@ -3137,13 +3137,13 @@
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="E80" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F80" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
@@ -3157,13 +3157,13 @@
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="E81" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F81" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
@@ -3177,13 +3177,13 @@
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="E82" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F82" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -3197,13 +3197,13 @@
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="E83" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F83" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
@@ -3217,13 +3217,13 @@
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="E84" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F84" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
@@ -3237,13 +3237,13 @@
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="E85" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F85" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
@@ -3257,13 +3257,13 @@
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="E86" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F86" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
@@ -3277,13 +3277,13 @@
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="E87" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F87" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
@@ -3297,13 +3297,13 @@
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="E88" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F88" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
@@ -3317,13 +3317,13 @@
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="E89" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F89" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
@@ -3337,13 +3337,13 @@
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="E90" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F90" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
@@ -3357,13 +3357,13 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="E91" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F91" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
@@ -3377,13 +3377,13 @@
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="E92" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F92" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
@@ -3397,13 +3397,13 @@
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E93" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F93" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
@@ -3417,13 +3417,13 @@
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="E94" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F94" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
@@ -3437,13 +3437,13 @@
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="E95" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F95" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
@@ -3457,13 +3457,13 @@
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="E96" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F96" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
@@ -3477,13 +3477,13 @@
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="E97" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F97" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
@@ -3497,13 +3497,13 @@
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="E98" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F98" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
@@ -3517,13 +3517,13 @@
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E99" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F99" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
@@ -3537,13 +3537,13 @@
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E100" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F100" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
@@ -3557,13 +3557,13 @@
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E101" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F101" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
@@ -3577,13 +3577,13 @@
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="E102" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F102" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
@@ -3597,13 +3597,13 @@
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="E103" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F103" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
@@ -3617,13 +3617,13 @@
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="E104" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="F104" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
@@ -3637,13 +3637,13 @@
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="E105" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="F105" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
@@ -3657,13 +3657,13 @@
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="E106" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F106" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
@@ -3677,13 +3677,13 @@
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="E107" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="F107" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
@@ -3697,13 +3697,13 @@
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="E108" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="F108" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
@@ -3717,13 +3717,13 @@
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E109" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="F109" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
@@ -3737,13 +3737,13 @@
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="E110" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F110" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
@@ -3757,13 +3757,13 @@
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="E111" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="F111" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
@@ -3777,13 +3777,13 @@
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="E112" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="F112" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
@@ -3797,13 +3797,13 @@
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E113" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="F113" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
@@ -3814,7 +3814,7 @@
         <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D114" t="s">
         <v>14</v>
@@ -3823,7 +3823,7 @@
         <v>14</v>
       </c>
       <c r="F114" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>